<commit_message>
Drools and some basic map rules
</commit_message>
<xml_diff>
--- a/doc/Rules.xlsx
+++ b/doc/Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="FlatMapRule" sheetId="2" r:id="rId1"/>
@@ -114,21 +114,12 @@
     <t>attr name</t>
   </si>
   <si>
-    <t>select value</t>
-  </si>
-  <si>
     <t>message</t>
   </si>
   <si>
     <t>[node]</t>
   </si>
   <si>
-    <t>AppendValueof</t>
-  </si>
-  <si>
-    <t>RemoveElementText</t>
-  </si>
-  <si>
     <t>SetAttributeValue</t>
   </si>
   <si>
@@ -136,6 +127,15 @@
   </si>
   <si>
     <t>Rule Model</t>
+  </si>
+  <si>
+    <t>replaceWithValueof</t>
+  </si>
+  <si>
+    <t>sourceElmNode</t>
+  </si>
+  <si>
+    <t>getNodeXslType</t>
   </si>
 </sst>
 </file>
@@ -694,21 +694,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.21875" style="4" customWidth="1"/>
-    <col min="2" max="3" width="19.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="24.28515625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="19.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -736,7 +736,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -750,7 +750,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -764,7 +764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -778,7 +778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -792,7 +792,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -806,7 +806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -820,7 +820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -834,7 +834,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -848,7 +848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -862,7 +862,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -876,7 +876,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -884,7 +884,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
@@ -892,7 +892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -900,7 +900,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -908,7 +908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -917,7 +917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
@@ -925,16 +925,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="D24" s="12"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>23</v>
       </c>
@@ -944,7 +944,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>24</v>
       </c>
@@ -954,64 +954,64 @@
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
     </row>
-    <row r="27" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>33</v>
-      </c>
       <c r="D27" s="16"/>
     </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>33</v>
-      </c>
       <c r="D28" s="19"/>
     </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="12"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="D31" s="16"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>31</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C32" s="14"/>
       <c r="D32" s="16"/>
     </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>29</v>

</xml_diff>